<commit_message>
Updated and added functions
Added a unique id for each event that is automatically assigned to each new event to differentiate between each one. Finished the del_Event() function. Added a function show_all_events() two display all events.
</commit_message>
<xml_diff>
--- a/my_Events.xlsx
+++ b/my_Events.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1680" yWindow="2055" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-25260" yWindow="2355" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="my_Events" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,12 +16,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -45,8 +53,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,76 +434,71 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="11.5703125" customWidth="1" min="1" max="1"/>
+    <col width="9.28515625" customWidth="1" min="4" max="4"/>
+    <col width="11.5703125" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>Day</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Month</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Year</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>22</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Birthday Tom</t>
-        </is>
-      </c>
+      <c r="A2" s="2" t="n"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15293965254512808429</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>05</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>2022</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Test2</t>
         </is>
@@ -502,48 +507,140 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>17779186155504800237</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>01</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>02</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Test3</t>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Test1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>18073954687356768749</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>04</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>2022</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Test2</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>13550180417212909</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>Test3</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>504221220135834093</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Test4</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1692833795598258669</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Test5</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="4294967293" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update, testing and planing
Added a reminder slot to in the excel and for the user to input when creating a event.

Next up:
Want: Implement a function check_events if todays date is the day the user want's to get reminded of a specific event.
Problem: We have to convert the information (day, month, year) from the excel Database to a date object.

I did this at the bottom of the code. Next is to implement the calculation for the reminder function and integrate the conversion into the function.
</commit_message>
<xml_diff>
--- a/my_Events.xlsx
+++ b/my_Events.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-25260" yWindow="2355" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="my_Events" sheetId="1" state="visible" r:id="rId1"/>
@@ -434,17 +434,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="11.5703125" customWidth="1" min="1" max="1"/>
     <col width="9.28515625" customWidth="1" min="4" max="4"/>
-    <col width="11.5703125" customWidth="1" min="5" max="5"/>
+    <col width="17.5703125" customWidth="1" min="5" max="5"/>
+    <col width="15.28515625" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -471,6 +472,11 @@
       <c r="E1" t="inlineStr">
         <is>
           <t>Description</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Reminder (days)</t>
         </is>
       </c>
     </row>
@@ -480,7 +486,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>11491406475739337197</t>
+          <t>3403722335677977069</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -502,6 +508,9 @@
         <is>
           <t>Mirek Geburtstag</t>
         </is>
+      </c>
+      <c r="F3" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: Form to create Event done
</commit_message>
<xml_diff>
--- a/my_Events.xlsx
+++ b/my_Events.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
@@ -543,6 +543,50 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>3667518741744194029</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Adrianas Bday</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1510441034453422573</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="4294967293" verticalDpi="0"/>

</xml_diff>

<commit_message>
Update: finished delete Event function
</commit_message>
<xml_diff>
--- a/my_Events.xlsx
+++ b/my_Events.xlsx
@@ -437,7 +437,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -516,17 +516,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>9710396847926677997</t>
+          <t>3667518741744194029</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>13</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>11</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -536,27 +536,29 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>TestEvent</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>5</v>
+          <t>Adrianas Bday</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3667518741744194029</t>
+          <t>8090963507605344749</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -564,28 +566,43 @@
           <t>2022</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Adrianas Bday</t>
-        </is>
-      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1510441034453422573</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
+          <t>9527163690503573997</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated method to display all Events
</commit_message>
<xml_diff>
--- a/my_Events.xlsx
+++ b/my_Events.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N13" sqref="N13"/>
@@ -604,6 +604,70 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>9691387881182728685</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Just a friendly reminder to enjoy your day</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2880808233611366893</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Test Event (Again)</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="4294967293" verticalDpi="0"/>

</xml_diff>

<commit_message>
Update: Upcoming Events now displayed in frame
</commit_message>
<xml_diff>
--- a/my_Events.xlsx
+++ b/my_Events.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N13" sqref="N13"/>
@@ -700,6 +700,134 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>13866811204960522733</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>16767335235704918509</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2064</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Dennis 63th Bday</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>17531903181772362221</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>TestEvent</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>13178649838081741293</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>TestEvent2</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="4294967293" verticalDpi="0"/>

</xml_diff>

<commit_message>
Update: display todays Events and Upcoming Events
</commit_message>
<xml_diff>
--- a/my_Events.xlsx
+++ b/my_Events.xlsx
@@ -59,7 +59,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -434,13 +434,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="F5" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col width="11.5703125" customWidth="1" min="1" max="1"/>
     <col width="9.28515625" customWidth="1" min="4" max="4"/>
@@ -486,7 +486,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3403722335677977069</t>
+          <t>4464960947490394605</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -506,325 +506,44 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Mirek Geburtstag</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>7</v>
+          <t>Papas Geburtstag</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3667518741744194029</t>
+          <t>8338478345572848109</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2065</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Adrianas Bday</t>
+          <t>Quatsch</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>14</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>8090963507605344749</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
           <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>9527163690503573997</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>9691387881182728685</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Just a friendly reminder to enjoy your day</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2880808233611366893</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Test Event (Again)</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>1270997458209346029</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>David Bday</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>13866811204960522733</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>16767335235704918509</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>09</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>2064</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Dennis 63th Bday</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>17531903181772362221</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>TestEvent</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>13178649838081741293</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>TestEvent2</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update: Added Messageboxes for add/delete buttons
</commit_message>
<xml_diff>
--- a/my_Events.xlsx
+++ b/my_Events.xlsx
@@ -518,12 +518,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>8338478345572848109</t>
+          <t>7264046483537334765</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>29</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -533,12 +533,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2065</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Quatsch</t>
+          <t>Ein Tag vor Berkos Bday</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">

</xml_diff>

<commit_message>
Update: Added Notifications, reworked all events
</commit_message>
<xml_diff>
--- a/my_Events.xlsx
+++ b/my_Events.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="A3:F5"/>
@@ -518,17 +518,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>7264046483537334765</t>
+          <t>7272754151794020845</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>08</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -538,12 +538,44 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Ein Tag vor Berkos Bday</t>
+          <t>Mamas Geburtstag</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>8252115886235587053</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Adrianas Geburtstag</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>10</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Build Exe command added to the README File
</commit_message>
<xml_diff>
--- a/my_Events.xlsx
+++ b/my_Events.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="A3:F5"/>
@@ -579,6 +579,102 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>15651062476621353453</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Rojan Haun</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>17017948802259489261</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>David Schelle geben</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>17846138601393754605</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Vincent Box'n</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="4294967293" verticalDpi="0"/>

</xml_diff>

<commit_message>
Update: implemented code for prepared Buttons
</commit_message>
<xml_diff>
--- a/my_Events.xlsx
+++ b/my_Events.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-23745" yWindow="3015" windowWidth="12150" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28800" yWindow="585" windowWidth="12150" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="all_Events" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -32,6 +32,13 @@
       <color theme="1"/>
       <sz val="11"/>
       <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="0"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -55,10 +62,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,10 +447,10 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B6" sqref="B6:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="11.5703125" customWidth="1" min="1" max="1"/>
     <col width="9.28515625" customWidth="1" min="4" max="4"/>
@@ -751,16 +759,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.140625" customWidth="1" min="1" max="1"/>
     <col width="14.28515625" customWidth="1" min="5" max="5"/>
+    <col width="15.85546875" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -795,8 +804,148 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="3" t="n"/>
+      <c r="B2" s="3" t="n"/>
+      <c r="C2" s="3" t="n"/>
+      <c r="D2" s="3" t="n"/>
+      <c r="E2" s="3" t="n"/>
+      <c r="F2" s="3" t="n"/>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>15651062476621353453</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Rojan Haun</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>17017948802259489261</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>David Schelle geben</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>7792422796411474413</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Another Test</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>13252142372198027757</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>What a Day</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="4294967293" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -806,13 +955,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="12.5703125" customWidth="1" min="1" max="1"/>
     <col width="16" customWidth="1" min="5" max="5"/>
@@ -850,6 +999,166 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>4464960947490394605</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Papas Geburtstag</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>4464960947490394605</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Papas Geburtstag</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>7272754151794020845</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Mamas Geburtstag</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>8252115886235587053</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Adrianas Geburtstag</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>17846138601393754605</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Vincent Box'n</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update: Removed preview text
</commit_message>
<xml_diff>
--- a/my_Events.xlsx
+++ b/my_Events.xlsx
@@ -444,13 +444,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col width="11.5703125" customWidth="1" min="1" max="1"/>
     <col width="9.28515625" customWidth="1" min="4" max="4"/>
@@ -744,6 +744,38 @@
       <c r="F10" t="inlineStr">
         <is>
           <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>3310658602400223725</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Nach Dänemark fahren</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -765,7 +797,7 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.140625" customWidth="1" min="1" max="1"/>
     <col width="14.28515625" customWidth="1" min="5" max="5"/>
@@ -961,7 +993,7 @@
       <selection activeCell="G3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="12.5703125" customWidth="1" min="1" max="1"/>
     <col width="16" customWidth="1" min="5" max="5"/>

</xml_diff>